<commit_message>
bump: version 0.21.0 → 0.21.1
</commit_message>
<xml_diff>
--- a/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
+++ b/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardjoe\OneDrive - Stichting Deltares\Documents\04. Deltares Projecten\04.160. EPIC Response Framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/ana_nunezsanchez_deltares_nl/Documents/Documents/Floods and Droughts/EPIC Response Tool/Software/Excel Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB61912B-4B5B-4132-8F73-6833B8832467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0E30048-5238-41C2-8119-CE758937D3A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agency_data" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,18 +42,9 @@
     <t>WRM Agency</t>
   </si>
   <si>
-    <t>Water Resource Management</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>Flood Risk Management</t>
-  </si>
-  <si>
-    <t>Drought Risk Management</t>
-  </si>
-  <si>
     <t>Integrated River Basin Planning</t>
   </si>
   <si>
@@ -103,9 +90,6 @@
     <t>DRM Agency</t>
   </si>
   <si>
-    <t>Disaster Risk Management</t>
-  </si>
-  <si>
     <t>Floodplain Regulation</t>
   </si>
   <si>
@@ -158,13 +142,25 @@
   </si>
   <si>
     <t xml:space="preserve">Social Protection </t>
+  </si>
+  <si>
+    <t>National Water Resource Management Sector Framework</t>
+  </si>
+  <si>
+    <t>Overarching Flood Risk Management Framework</t>
+  </si>
+  <si>
+    <t>Overarching National Drought Risk Management Framework</t>
+  </si>
+  <si>
+    <t>National Disaster Risk Management Sector Framework</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1000,17 +996,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1021,433 +1017,433 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
         <v>21</v>
       </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>22</v>
       </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>22</v>
       </c>
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
         <v>30</v>
       </c>
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
         <v>31</v>
       </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" t="s">
         <v>32</v>
       </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>33</v>
       </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="B39" t="s">
         <v>36</v>
       </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>37</v>
       </c>
-      <c r="B37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>41</v>
-      </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1457,6 +1453,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1465,17 +1467,11 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008FD03EABF3F2FB448DAE5CD2CE5D353B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="98b843f414b1d31b21b2b135980a1ce8">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be3c9163-79a1-42b6-a061-0833e6c3add8" xmlns:ns4="4e51305d-5de6-45a6-8f4b-ddcbc1e897ba" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed93da940882836d4864d93d9a5709d2" ns3:_="" ns4:_="">
-    <xsd:import namespace="be3c9163-79a1-42b6-a061-0833e6c3add8"/>
-    <xsd:import namespace="4e51305d-5de6-45a6-8f4b-ddcbc1e897ba"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004CF95EF2F384F0419312B394CBDE3AE2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31f6efdc87a01d4ba6154ecd9afe69b2">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="18fba281-3140-4e33-b78f-87df0c1efb23" xmlns:ns4="f7620e32-1325-4c29-861c-5840d24c4310" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef933d5bbd2bd3eb58c8ad997b164a29" ns3:_="" ns4:_="">
+    <xsd:import namespace="18fba281-3140-4e33-b78f-87df0c1efb23"/>
+    <xsd:import namespace="f7620e32-1325-4c29-861c-5840d24c4310"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -1484,15 +1480,15 @@
               <xsd:all>
                 <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
@@ -1503,7 +1499,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="be3c9163-79a1-42b6-a061-0833e6c3add8" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="18fba281-3140-4e33-b78f-87df0c1efb23" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -1516,34 +1512,34 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="13" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="16" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -1566,10 +1562,10 @@
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4e51305d-5de6-45a6-8f4b-ddcbc1e897ba" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f7620e32-1325-4c29-861c-5840d24c4310" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -1588,14 +1584,14 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="SharingHintHash" ma:index="12" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+    <xsd:element name="SharingHintHash" ma:index="18" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -1701,13 +1697,45 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E416E2-4A6A-4C1B-B794-2BED7D3C2983}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="18fba281-3140-4e33-b78f-87df0c1efb23"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f7620e32-1325-4c29-861c-5840d24c4310"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E416E2-4A6A-4C1B-B794-2BED7D3C2983}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EF0128B-7804-47D5-B4F5-3E11AFB6EF0E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4171F17E-5F2A-4728-82FF-84EE42ECDF4B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="18fba281-3140-4e33-b78f-87df0c1efb23"/>
+    <ds:schemaRef ds:uri="f7620e32-1325-4c29-861c-5840d24c4310"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
patch(question_importer.py): Fixed first after 'get' on a program query
</commit_message>
<xml_diff>
--- a/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
+++ b/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/ana_nunezsanchez_deltares_nl/Documents/Documents/Floods and Droughts/EPIC Response Tool/Software/Excel Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0E30048-5238-41C2-8119-CE758937D3A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A829962D-D2BC-4DF3-BBFE-A0F086FA7A93}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10110" yWindow="1890" windowWidth="16800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agency_data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
   <si>
     <t>Agency</t>
   </si>
@@ -100,21 +100,6 @@
   </si>
   <si>
     <t>National Framework for NMS/NHS Services</t>
-  </si>
-  <si>
-    <t>National Water Data Program</t>
-  </si>
-  <si>
-    <t>Drought Monitoring and Impact Assessment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flood Forecasting and Warning </t>
-  </si>
-  <si>
-    <t>Agrometeorological Advisory Services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National Climate Assessment </t>
   </si>
   <si>
     <t>Agriculture</t>
@@ -994,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1022,7 +1007,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1033,7 +1018,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1044,7 +1029,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1198,7 +1183,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1209,7 +1194,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -1286,7 +1271,7 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -1294,10 +1279,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -1305,10 +1290,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -1316,10 +1301,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -1327,10 +1312,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -1338,10 +1323,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -1349,10 +1334,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
         <v>29</v>
-      </c>
-      <c r="B32" t="s">
-        <v>40</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -1360,10 +1345,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -1371,10 +1356,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -1382,67 +1367,12 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1453,21 +1383,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004CF95EF2F384F0419312B394CBDE3AE2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31f6efdc87a01d4ba6154ecd9afe69b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="18fba281-3140-4e33-b78f-87df0c1efb23" xmlns:ns4="f7620e32-1325-4c29-861c-5840d24c4310" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef933d5bbd2bd3eb58c8ad997b164a29" ns3:_="" ns4:_="">
     <xsd:import namespace="18fba281-3140-4e33-b78f-87df0c1efb23"/>
@@ -1696,32 +1611,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="18fba281-3140-4e33-b78f-87df0c1efb23"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f7620e32-1325-4c29-861c-5840d24c4310"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E416E2-4A6A-4C1B-B794-2BED7D3C2983}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4171F17E-5F2A-4728-82FF-84EE42ECDF4B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1738,4 +1643,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E416E2-4A6A-4C1B-B794-2BED7D3C2983}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="18fba281-3140-4e33-b78f-87df0c1efb23"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f7620e32-1325-4c29-861c-5840d24c4310"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
test(test_datda/xlsx): Updated data with client's questions.
</commit_message>
<xml_diff>
--- a/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
+++ b/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\originals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A829962D-D2BC-4DF3-BBFE-A0F086FA7A93}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAA82A5-3887-4767-81A8-8FB45144FCE0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10110" yWindow="1890" windowWidth="16800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12165" yWindow="2175" windowWidth="16800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agency_data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="38">
   <si>
     <t>Agency</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>National Disaster Risk Management Sector Framework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Co-Production of Services </t>
   </si>
 </sst>
 </file>
@@ -981,17 +984,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1013,7 +1016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1024,7 +1027,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1035,7 +1038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1057,7 +1060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1079,7 +1082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1156,7 +1159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1167,7 +1170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1178,7 +1181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1189,7 +1192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1200,7 +1203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1211,7 +1214,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1222,7 +1225,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1233,7 +1236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1244,7 +1247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1255,7 +1258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1266,18 +1269,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1299,7 +1302,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -1310,7 +1313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -1321,7 +1324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -1332,7 +1335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -1343,7 +1346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -1354,7 +1357,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1365,7 +1368,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -1383,6 +1386,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004CF95EF2F384F0419312B394CBDE3AE2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31f6efdc87a01d4ba6154ecd9afe69b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="18fba281-3140-4e33-b78f-87df0c1efb23" xmlns:ns4="f7620e32-1325-4c29-861c-5840d24c4310" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef933d5bbd2bd3eb58c8ad997b164a29" ns3:_="" ns4:_="">
     <xsd:import namespace="18fba281-3140-4e33-b78f-87df0c1efb23"/>
@@ -1611,7 +1620,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1620,13 +1629,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="18fba281-3140-4e33-b78f-87df0c1efb23"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f7620e32-1325-4c29-861c-5840d24c4310"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4171F17E-5F2A-4728-82FF-84EE42ECDF4B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1645,27 +1665,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E416E2-4A6A-4C1B-B794-2BED7D3C2983}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="18fba281-3140-4e33-b78f-87df0c1efb23"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f7620e32-1325-4c29-861c-5840d24c4310"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Feature/67 add reference and reference link as fields for program (#68)
* feat(xlsx/domain_importer.py;models.py;program_serializer.py): Added new fields for Program

* patch(domain_importer.py): Fixed domain_importer and extended related tests

* ci(initial_epic_data.xlsx): Updated domain data

* bump: version 0.21.1 → 0.22.0

* test(test_datda/xlsx): Updated data with client's questions.

* test(test_question_importer.py): Fixed failing tests
</commit_message>
<xml_diff>
--- a/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
+++ b/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\originals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A829962D-D2BC-4DF3-BBFE-A0F086FA7A93}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAA82A5-3887-4767-81A8-8FB45144FCE0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10110" yWindow="1890" windowWidth="16800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12165" yWindow="2175" windowWidth="16800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agency_data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="38">
   <si>
     <t>Agency</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>National Disaster Risk Management Sector Framework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Co-Production of Services </t>
   </si>
 </sst>
 </file>
@@ -981,17 +984,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1013,7 +1016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1024,7 +1027,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1035,7 +1038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1057,7 +1060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1079,7 +1082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1156,7 +1159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1167,7 +1170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1178,7 +1181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1189,7 +1192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1200,7 +1203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1211,7 +1214,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1222,7 +1225,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1233,7 +1236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1244,7 +1247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1255,7 +1258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1266,18 +1269,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1299,7 +1302,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -1310,7 +1313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -1321,7 +1324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -1332,7 +1335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -1343,7 +1346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -1354,7 +1357,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1365,7 +1368,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -1383,6 +1386,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004CF95EF2F384F0419312B394CBDE3AE2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31f6efdc87a01d4ba6154ecd9afe69b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="18fba281-3140-4e33-b78f-87df0c1efb23" xmlns:ns4="f7620e32-1325-4c29-861c-5840d24c4310" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef933d5bbd2bd3eb58c8ad997b164a29" ns3:_="" ns4:_="">
     <xsd:import namespace="18fba281-3140-4e33-b78f-87df0c1efb23"/>
@@ -1611,7 +1620,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1620,13 +1629,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="18fba281-3140-4e33-b78f-87df0c1efb23"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f7620e32-1325-4c29-861c-5840d24c4310"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4171F17E-5F2A-4728-82FF-84EE42ECDF4B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1645,27 +1665,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E416E2-4A6A-4C1B-B794-2BED7D3C2983}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="18fba281-3140-4e33-b78f-87df0c1efb23"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f7620e32-1325-4c29-861c-5840d24c4310"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore: Updated xlsx files and related tests
</commit_message>
<xml_diff>
--- a/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
+++ b/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\originals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAA82A5-3887-4767-81A8-8FB45144FCE0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7710A19A-F0BB-4032-8D67-EAAB8E2D31F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12165" yWindow="2175" windowWidth="16800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14070" yWindow="585" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agency_data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="50">
   <si>
     <t>Agency</t>
   </si>
@@ -42,9 +42,36 @@
     <t>WRM Agency</t>
   </si>
   <si>
+    <t>National Water Resource Management Sector Framework</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
+    <t>Overarching Flood Risk Management Framework</t>
+  </si>
+  <si>
+    <t>Overarching National Drought Risk Management Framework</t>
+  </si>
+  <si>
+    <t>Local Government</t>
+  </si>
+  <si>
+    <t>Public Participation &amp; Stakeholder Engagement</t>
+  </si>
+  <si>
+    <t>Social Inclusion</t>
+  </si>
+  <si>
+    <t>Education &amp; Risk Communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scientific Collaboration </t>
+  </si>
+  <si>
+    <t>Open Data</t>
+  </si>
+  <si>
     <t>Integrated River Basin Planning</t>
   </si>
   <si>
@@ -90,9 +117,18 @@
     <t>DRM Agency</t>
   </si>
   <si>
+    <t>National Disaster Risk Management Sector Framework</t>
+  </si>
+  <si>
+    <t>Local Flood Mitigation Planning</t>
+  </si>
+  <si>
     <t>Floodplain Regulation</t>
   </si>
   <si>
+    <t>Flood Emergency Preparedness, Response, and Relief</t>
+  </si>
+  <si>
     <t>Flood Disaster Recovery</t>
   </si>
   <si>
@@ -108,6 +144,9 @@
     <t>Agriculture Policies and Climate Smart Agriculture</t>
   </si>
   <si>
+    <t>Watershed Management</t>
+  </si>
+  <si>
     <t>Agriculture Drought Response</t>
   </si>
   <si>
@@ -129,19 +168,16 @@
     <t xml:space="preserve">Social Protection </t>
   </si>
   <si>
-    <t>National Water Resource Management Sector Framework</t>
-  </si>
-  <si>
-    <t>Overarching Flood Risk Management Framework</t>
-  </si>
-  <si>
-    <t>Overarching National Drought Risk Management Framework</t>
-  </si>
-  <si>
-    <t>National Disaster Risk Management Sector Framework</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Co-Production of Services </t>
+    <t>Finance Agency</t>
+  </si>
+  <si>
+    <t>Co-Production of Services</t>
+  </si>
+  <si>
+    <t>Disaster Risk Financing Instruments</t>
+  </si>
+  <si>
+    <t>Disaster Risk Financing National Sector Framework</t>
   </si>
 </sst>
 </file>
@@ -284,7 +320,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,6 +498,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -625,8 +667,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -982,19 +1025,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1005,359 +1048,323 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
         <v>13</v>
       </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1365,18 +1372,452 @@
         <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" t="s">
         <v>27</v>
       </c>
-      <c r="C35" t="s">
-        <v>4</v>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>36</v>
+      </c>
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>36</v>
+      </c>
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>41</v>
+      </c>
+      <c r="B63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>41</v>
+      </c>
+      <c r="B66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" t="s">
+        <v>43</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>41</v>
+      </c>
+      <c r="B69" t="s">
+        <v>38</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>45</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>45</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>45</v>
+      </c>
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>45</v>
+      </c>
+      <c r="B73" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>45</v>
+      </c>
+      <c r="B74" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>45</v>
+      </c>
+      <c r="B75" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>45</v>
+      </c>
+      <c r="B76" t="s">
+        <v>40</v>
+      </c>
+      <c r="C76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>46</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>46</v>
+      </c>
+      <c r="B78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>46</v>
+      </c>
+      <c r="B79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>46</v>
+      </c>
+      <c r="B80" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>46</v>
+      </c>
+      <c r="B81" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>46</v>
+      </c>
+      <c r="B82" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>46</v>
+      </c>
+      <c r="B83" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>46</v>
+      </c>
+      <c r="B84" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1632,16 +2073,8 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="18fba281-3140-4e33-b78f-87df0c1efb23"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f7620e32-1325-4c29-861c-5840d24c4310"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Chore/update xlsx files (#84)
* chore: Updated xlsx files and related tests

* bump: version 0.27.0 → 0.27.1
</commit_message>
<xml_diff>
--- a/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
+++ b/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\originals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAA82A5-3887-4767-81A8-8FB45144FCE0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7710A19A-F0BB-4032-8D67-EAAB8E2D31F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12165" yWindow="2175" windowWidth="16800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14070" yWindow="585" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agency_data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="50">
   <si>
     <t>Agency</t>
   </si>
@@ -42,9 +42,36 @@
     <t>WRM Agency</t>
   </si>
   <si>
+    <t>National Water Resource Management Sector Framework</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
+    <t>Overarching Flood Risk Management Framework</t>
+  </si>
+  <si>
+    <t>Overarching National Drought Risk Management Framework</t>
+  </si>
+  <si>
+    <t>Local Government</t>
+  </si>
+  <si>
+    <t>Public Participation &amp; Stakeholder Engagement</t>
+  </si>
+  <si>
+    <t>Social Inclusion</t>
+  </si>
+  <si>
+    <t>Education &amp; Risk Communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scientific Collaboration </t>
+  </si>
+  <si>
+    <t>Open Data</t>
+  </si>
+  <si>
     <t>Integrated River Basin Planning</t>
   </si>
   <si>
@@ -90,9 +117,18 @@
     <t>DRM Agency</t>
   </si>
   <si>
+    <t>National Disaster Risk Management Sector Framework</t>
+  </si>
+  <si>
+    <t>Local Flood Mitigation Planning</t>
+  </si>
+  <si>
     <t>Floodplain Regulation</t>
   </si>
   <si>
+    <t>Flood Emergency Preparedness, Response, and Relief</t>
+  </si>
+  <si>
     <t>Flood Disaster Recovery</t>
   </si>
   <si>
@@ -108,6 +144,9 @@
     <t>Agriculture Policies and Climate Smart Agriculture</t>
   </si>
   <si>
+    <t>Watershed Management</t>
+  </si>
+  <si>
     <t>Agriculture Drought Response</t>
   </si>
   <si>
@@ -129,19 +168,16 @@
     <t xml:space="preserve">Social Protection </t>
   </si>
   <si>
-    <t>National Water Resource Management Sector Framework</t>
-  </si>
-  <si>
-    <t>Overarching Flood Risk Management Framework</t>
-  </si>
-  <si>
-    <t>Overarching National Drought Risk Management Framework</t>
-  </si>
-  <si>
-    <t>National Disaster Risk Management Sector Framework</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Co-Production of Services </t>
+    <t>Finance Agency</t>
+  </si>
+  <si>
+    <t>Co-Production of Services</t>
+  </si>
+  <si>
+    <t>Disaster Risk Financing Instruments</t>
+  </si>
+  <si>
+    <t>Disaster Risk Financing National Sector Framework</t>
   </si>
 </sst>
 </file>
@@ -284,7 +320,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,6 +498,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -625,8 +667,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -982,19 +1025,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1005,359 +1048,323 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
         <v>13</v>
       </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1365,18 +1372,452 @@
         <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" t="s">
         <v>27</v>
       </c>
-      <c r="C35" t="s">
-        <v>4</v>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>36</v>
+      </c>
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>36</v>
+      </c>
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>41</v>
+      </c>
+      <c r="B63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>41</v>
+      </c>
+      <c r="B66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" t="s">
+        <v>43</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>41</v>
+      </c>
+      <c r="B69" t="s">
+        <v>38</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>45</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>45</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>45</v>
+      </c>
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>45</v>
+      </c>
+      <c r="B73" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>45</v>
+      </c>
+      <c r="B74" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>45</v>
+      </c>
+      <c r="B75" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>45</v>
+      </c>
+      <c r="B76" t="s">
+        <v>40</v>
+      </c>
+      <c r="C76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>46</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>46</v>
+      </c>
+      <c r="B78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>46</v>
+      </c>
+      <c r="B79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>46</v>
+      </c>
+      <c r="B80" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>46</v>
+      </c>
+      <c r="B81" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>46</v>
+      </c>
+      <c r="B82" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>46</v>
+      </c>
+      <c r="B83" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>46</v>
+      </c>
+      <c r="B84" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1632,16 +2073,8 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="18fba281-3140-4e33-b78f-87df0c1efb23"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f7620e32-1325-4c29-861c-5840d24c4310"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
docs(xlsx): Updated domain data and related tests
</commit_message>
<xml_diff>
--- a/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
+++ b/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7710A19A-F0BB-4032-8D67-EAAB8E2D31F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E5D0EA-23E3-42DE-9DBB-7D9DA9D9AC32}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14070" yWindow="585" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agency_data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="49">
   <si>
     <t>Agency</t>
   </si>
@@ -174,10 +174,7 @@
     <t>Co-Production of Services</t>
   </si>
   <si>
-    <t>Disaster Risk Financing Instruments</t>
-  </si>
-  <si>
-    <t>Disaster Risk Financing National Sector Framework</t>
+    <t>Disaster Risk Financing National Sector Framework and Instruments</t>
   </si>
 </sst>
 </file>
@@ -1025,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83:XFD83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1812,14 +1809,6 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>46</v>
-      </c>
-      <c r="B84" t="s">
-        <v>49</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1827,9 +1816,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2062,19 +2054,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E416E2-4A6A-4C1B-B794-2BED7D3C2983}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2099,9 +2087,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E416E2-4A6A-4C1B-B794-2BED7D3C2983}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Chore/update xlsx files (#85)
* chore: Updated xlsx files and related tests

* bump: version 0.27.0 → 0.27.1

* docs(xlsx): Updated domain data and related tests
</commit_message>
<xml_diff>
--- a/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
+++ b/backend/epic_app/tests/test_data/xlsx/agency_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7710A19A-F0BB-4032-8D67-EAAB8E2D31F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E5D0EA-23E3-42DE-9DBB-7D9DA9D9AC32}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14070" yWindow="585" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agency_data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="49">
   <si>
     <t>Agency</t>
   </si>
@@ -174,10 +174,7 @@
     <t>Co-Production of Services</t>
   </si>
   <si>
-    <t>Disaster Risk Financing Instruments</t>
-  </si>
-  <si>
-    <t>Disaster Risk Financing National Sector Framework</t>
+    <t>Disaster Risk Financing National Sector Framework and Instruments</t>
   </si>
 </sst>
 </file>
@@ -1025,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83:XFD83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1812,14 +1809,6 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>46</v>
-      </c>
-      <c r="B84" t="s">
-        <v>49</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1827,9 +1816,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2062,19 +2054,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E416E2-4A6A-4C1B-B794-2BED7D3C2983}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2099,9 +2087,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E416E2-4A6A-4C1B-B794-2BED7D3C2983}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>